<commit_message>
All the excel dataframes and the excel file
</commit_message>
<xml_diff>
--- a/data/vaccine-distribution-data.xlsx
+++ b/data/vaccine-distribution-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aalto Courses\Database\Project_Vaccination\cs-a-1153-2022-project-vaccine-distribution-group-21\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7705572A-9BE6-4E5D-A26F-670AE034AF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DFF11A-95B8-468D-8274-D73B604E0B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VaccineType" sheetId="1" r:id="rId1"/>
@@ -3655,7 +3655,7 @@
   </sheetPr>
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -9026,7 +9026,7 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -13983,7 +13983,7 @@
   <customSheetViews>
     <customSheetView guid="{54DCABD8-C2F3-4655-B3D2-F93603271522}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="F1:F1000" xr:uid="{92E629A8-823F-4C24-9ECB-A7A8724B9395}"/>
+      <autoFilter ref="F1:F1000" xr:uid="{FC34E73A-9300-4067-BD18-8F99EA92BDAC}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>